<commit_message>
`Added new features and functionality to student-attendance application`
</commit_message>
<xml_diff>
--- a/student-attendance/scripts/Students/I-II ECE A  Name list.xlsx
+++ b/student-attendance/scripts/Students/I-II ECE A  Name list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\SANGEETHA\SYSTEM2\2025-26 EVEN SEM DETAILS\CNW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\Attendence-Application\student-attendance\scripts\Students\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB71F33F-DABE-4C87-8EC3-DB77EA891B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ECE A" sheetId="1" r:id="rId1"/>
@@ -245,7 +246,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -341,9 +342,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -354,9 +352,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -369,31 +364,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -689,33 +670,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,1081 +713,1086 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
+        <v>100101191251030</v>
+      </c>
+      <c r="C3" s="3">
+        <v>622125105001</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
         <v>100101191251139</v>
       </c>
-      <c r="C3" s="4">
-        <v>622125105001</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="C4" s="3">
+        <v>622125105002</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
         <v>100121191251031</v>
       </c>
-      <c r="C4" s="4">
-        <v>622125105002</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>100101191251135</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>622125105003</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>100221191251016</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="3">
+        <v>100101191251135</v>
+      </c>
+      <c r="C6" s="3">
         <v>622125105004</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
-        <v>100101191251085</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="3">
+        <v>100221191251016</v>
+      </c>
+      <c r="C7" s="3">
         <v>622125105005</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
-        <v>100101191251179</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" s="3">
+        <v>100101191251085</v>
+      </c>
+      <c r="C8" s="3">
         <v>622125105006</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
-        <v>100101191251134</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="3">
+        <v>100101191251179</v>
+      </c>
+      <c r="C9" s="3">
         <v>622125105007</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
-        <v>100121191251055</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="3">
+        <v>100101191251134</v>
+      </c>
+      <c r="C10" s="3">
         <v>622125105008</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
-        <v>100101191251103</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" s="3">
+        <v>100121191251055</v>
+      </c>
+      <c r="C11" s="3">
         <v>622125105009</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
-        <v>100101191251128</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="B12" s="3">
+        <v>100101191251103</v>
+      </c>
+      <c r="C12" s="3">
         <v>622125105010</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
-        <v>100101191251152</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B13" s="3">
+        <v>100101191251128</v>
+      </c>
+      <c r="C13" s="3">
         <v>622125105011</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="4">
-        <v>100221191251010</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="B14" s="3">
+        <v>100101191251152</v>
+      </c>
+      <c r="C14" s="3">
         <v>622125105012</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="4">
-        <v>100101191251247</v>
-      </c>
-      <c r="C15" s="4">
+      <c r="B15" s="3">
+        <v>100221191251010</v>
+      </c>
+      <c r="C15" s="3">
         <v>622125105013</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="4">
-        <v>100101191251065</v>
-      </c>
-      <c r="C16" s="4">
+      <c r="B16" s="3">
+        <v>100101191251247</v>
+      </c>
+      <c r="C16" s="3">
         <v>622125105014</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="4">
-        <v>100101191251182</v>
-      </c>
-      <c r="C17" s="4">
+      <c r="B17" s="3">
+        <v>100101191251065</v>
+      </c>
+      <c r="C17" s="3">
         <v>622125105015</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="4">
-        <v>100101191251143</v>
-      </c>
-      <c r="C18" s="4">
+      <c r="B18" s="3">
+        <v>100101191251182</v>
+      </c>
+      <c r="C18" s="3">
         <v>622125105016</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="4">
-        <v>100221191251019</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="B19" s="3">
+        <v>100101191251143</v>
+      </c>
+      <c r="C19" s="3">
         <v>622125105017</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="4">
-        <v>100101191251072</v>
-      </c>
-      <c r="C20" s="4">
+      <c r="B20" s="3">
+        <v>100221191251019</v>
+      </c>
+      <c r="C20" s="3">
         <v>622125105018</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="4">
-        <v>100101191251169</v>
-      </c>
-      <c r="C21" s="4">
+      <c r="B21" s="3">
+        <v>100101191251072</v>
+      </c>
+      <c r="C21" s="3">
         <v>622125105019</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="4">
-        <v>100101191251141</v>
-      </c>
-      <c r="C22" s="4">
+      <c r="B22" s="3">
+        <v>100101191251169</v>
+      </c>
+      <c r="C22" s="3">
         <v>622125105020</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="4">
-        <v>100121191251057</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="B23" s="3">
+        <v>100101191251141</v>
+      </c>
+      <c r="C23" s="3">
         <v>622125105021</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="4">
-        <v>100101191251137</v>
-      </c>
-      <c r="C24" s="4">
+      <c r="B24" s="3">
+        <v>100121191251057</v>
+      </c>
+      <c r="C24" s="3">
         <v>622125105022</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="4">
-        <v>100101191251219</v>
-      </c>
-      <c r="C25" s="4">
+      <c r="B25" s="3">
+        <v>100101191251137</v>
+      </c>
+      <c r="C25" s="3">
         <v>622125105023</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="4">
-        <v>100101191251188</v>
-      </c>
-      <c r="C26" s="4">
+      <c r="B26" s="3">
+        <v>100101191251219</v>
+      </c>
+      <c r="C26" s="3">
         <v>622125105024</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="4">
-        <v>100121191251038</v>
-      </c>
-      <c r="C27" s="4">
+      <c r="B27" s="3">
+        <v>100101191251188</v>
+      </c>
+      <c r="C27" s="3">
         <v>622125105025</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="4">
-        <v>100101191251123</v>
-      </c>
-      <c r="C28" s="4">
+      <c r="B28" s="3">
+        <v>100121191251038</v>
+      </c>
+      <c r="C28" s="3">
         <v>622125105026</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="4">
-        <v>100101191251158</v>
-      </c>
-      <c r="C29" s="4">
+      <c r="B29" s="3">
+        <v>100101191251123</v>
+      </c>
+      <c r="C29" s="3">
         <v>622125105027</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="4">
-        <v>100101191251226</v>
-      </c>
-      <c r="C30" s="4">
+      <c r="B30" s="3">
+        <v>100101191251158</v>
+      </c>
+      <c r="C30" s="3">
         <v>622125105028</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="4">
-        <v>100101191251048</v>
-      </c>
-      <c r="C31" s="4">
+      <c r="B31" s="3">
+        <v>100101191251226</v>
+      </c>
+      <c r="C31" s="3">
         <v>622125105029</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="4">
-        <v>100101191251097</v>
-      </c>
-      <c r="C32" s="4">
+      <c r="B32" s="3">
+        <v>100101191251048</v>
+      </c>
+      <c r="C32" s="3">
         <v>622125105030</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="4">
-        <v>100101191251162</v>
-      </c>
-      <c r="C33" s="4">
+      <c r="B33" s="3">
+        <v>100101191251097</v>
+      </c>
+      <c r="C33" s="3">
         <v>622125105031</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="4">
-        <v>100101191251059</v>
-      </c>
-      <c r="C34" s="4">
+      <c r="B34" s="3">
+        <v>100101191251162</v>
+      </c>
+      <c r="C34" s="3">
         <v>622125105032</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="4">
-        <v>100101191251056</v>
-      </c>
-      <c r="C35" s="4">
+      <c r="B35" s="3">
+        <v>100101191251059</v>
+      </c>
+      <c r="C35" s="3">
         <v>622125105033</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="4">
-        <v>100221191251012</v>
-      </c>
-      <c r="C36" s="4">
+      <c r="B36" s="3">
+        <v>100101191251056</v>
+      </c>
+      <c r="C36" s="3">
         <v>622125105034</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="4">
-        <v>100221191251015</v>
-      </c>
-      <c r="C37" s="4">
+      <c r="B37" s="3">
+        <v>100221191251012</v>
+      </c>
+      <c r="C37" s="3">
         <v>622125105035</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="4">
-        <v>100101191251205</v>
-      </c>
-      <c r="C38" s="4">
+      <c r="B38" s="3">
+        <v>100221191251015</v>
+      </c>
+      <c r="C38" s="3">
         <v>622125105036</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="4">
-        <v>100101191251177</v>
-      </c>
-      <c r="C39" s="4">
+      <c r="B39" s="3">
+        <v>100101191251205</v>
+      </c>
+      <c r="C39" s="3">
         <v>622125105037</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="4">
-        <v>100101191251151</v>
-      </c>
-      <c r="C40" s="4">
+      <c r="B40" s="3">
+        <v>100101191251177</v>
+      </c>
+      <c r="C40" s="3">
         <v>622125105038</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="4">
-        <v>100101191251232</v>
-      </c>
-      <c r="C41" s="4">
+      <c r="B41" s="3">
+        <v>100101191251151</v>
+      </c>
+      <c r="C41" s="3">
         <v>622125105039</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="4">
-        <v>100101191251093</v>
-      </c>
-      <c r="C42" s="4">
+      <c r="B42" s="3">
+        <v>100101191251232</v>
+      </c>
+      <c r="C42" s="3">
         <v>622125105040</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="4">
-        <v>100121191251059</v>
-      </c>
-      <c r="C43" s="4">
+      <c r="B43" s="3">
+        <v>100101191251093</v>
+      </c>
+      <c r="C43" s="3">
         <v>622125105041</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E43" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="4">
-        <v>100101191251104</v>
-      </c>
-      <c r="C44" s="4">
+      <c r="B44" s="3">
+        <v>100121191251059</v>
+      </c>
+      <c r="C44" s="3">
         <v>622125105042</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E44" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E44" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" s="4">
-        <v>100121191251066</v>
-      </c>
-      <c r="C45" s="4">
+      <c r="B45" s="3">
+        <v>100101191251104</v>
+      </c>
+      <c r="C45" s="3">
         <v>622125105043</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E45" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E45" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="4">
-        <v>100121191251063</v>
-      </c>
-      <c r="C46" s="4">
+      <c r="B46" s="3">
+        <v>100121191251066</v>
+      </c>
+      <c r="C46" s="3">
         <v>622125105044</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="4">
-        <v>100121191251005</v>
-      </c>
-      <c r="C47" s="4">
+      <c r="B47" s="3">
+        <v>100121191251063</v>
+      </c>
+      <c r="C47" s="3">
         <v>622125105045</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E47" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E47" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="4">
-        <v>100121191251054</v>
-      </c>
-      <c r="C48" s="4">
+      <c r="B48" s="3">
+        <v>100121191251005</v>
+      </c>
+      <c r="C48" s="3">
         <v>622125105046</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E48" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="4">
-        <v>100101191251026</v>
-      </c>
-      <c r="C49" s="4">
+      <c r="B49" s="3">
+        <v>100121191251054</v>
+      </c>
+      <c r="C49" s="3">
         <v>622125105047</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E49" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="B50" s="4">
-        <v>100101191251003</v>
-      </c>
-      <c r="C50" s="4">
+      <c r="B50" s="3">
+        <v>100101191251026</v>
+      </c>
+      <c r="C50" s="3">
         <v>622125105048</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E50" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E50" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="4">
-        <v>100101191251170</v>
-      </c>
-      <c r="C51" s="4">
+      <c r="B51" s="3">
+        <v>100101191251003</v>
+      </c>
+      <c r="C51" s="3">
         <v>622125105049</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E51" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E51" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="4">
-        <v>100121191251039</v>
-      </c>
-      <c r="C52" s="4">
+      <c r="B52" s="3">
+        <v>100101191251170</v>
+      </c>
+      <c r="C52" s="3">
         <v>622125105050</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E52" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E52" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>51</v>
       </c>
-      <c r="B53" s="4">
-        <v>100101191251246</v>
-      </c>
-      <c r="C53" s="4">
+      <c r="B53" s="3">
+        <v>100121191251039</v>
+      </c>
+      <c r="C53" s="3">
         <v>622125105051</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E53" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E53" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="4">
-        <v>100101191251235</v>
-      </c>
-      <c r="C54" s="4">
+      <c r="B54" s="3">
+        <v>100101191251246</v>
+      </c>
+      <c r="C54" s="3">
         <v>622125105052</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E54" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="4">
-        <v>100121191251022</v>
-      </c>
-      <c r="C55" s="4">
+      <c r="B55" s="3">
+        <v>100101191251235</v>
+      </c>
+      <c r="C55" s="3">
         <v>622125105053</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E55" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="4">
-        <v>100101191251156</v>
-      </c>
-      <c r="C56" s="4">
+      <c r="B56" s="3">
+        <v>100121191251022</v>
+      </c>
+      <c r="C56" s="3">
         <v>622125105054</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E56" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="4">
-        <v>100121191251067</v>
-      </c>
-      <c r="C57" s="4">
+      <c r="B57" s="3">
+        <v>100101191251156</v>
+      </c>
+      <c r="C57" s="3">
         <v>622125105055</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E57" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="4">
-        <v>100101191251167</v>
-      </c>
-      <c r="C58" s="4">
+      <c r="B58" s="3">
+        <v>100121191251067</v>
+      </c>
+      <c r="C58" s="3">
         <v>622125105056</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="4">
-        <v>100101191251149</v>
-      </c>
-      <c r="C59" s="4">
+      <c r="B59" s="3">
+        <v>100101191251167</v>
+      </c>
+      <c r="C59" s="3">
         <v>622125105057</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E59" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="4">
-        <v>100101191251240</v>
-      </c>
-      <c r="C60" s="4">
+      <c r="B60" s="3">
+        <v>100101191251149</v>
+      </c>
+      <c r="C60" s="3">
         <v>622125105058</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E60" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="4">
-        <v>100101191251224</v>
-      </c>
-      <c r="C61" s="4">
+      <c r="B61" s="3">
+        <v>100101191251240</v>
+      </c>
+      <c r="C61" s="3">
         <v>622125105059</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E61" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="4">
-        <v>100101191251147</v>
-      </c>
-      <c r="C62" s="4">
+      <c r="B62" s="3">
+        <v>100101191251224</v>
+      </c>
+      <c r="C62" s="3">
         <v>622125105060</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E62" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="4">
-        <v>100121191251051</v>
-      </c>
-      <c r="C63" s="4">
+      <c r="B63" s="3">
+        <v>100101191251147</v>
+      </c>
+      <c r="C63" s="3">
         <v>622125105061</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E63" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="4">
-        <v>100101191251161</v>
-      </c>
-      <c r="C64" s="4">
+      <c r="B64" s="3">
+        <v>100121191251051</v>
+      </c>
+      <c r="C64" s="3">
         <v>622125105062</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E64" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E64" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="8"/>
-      <c r="C65" s="4">
+      <c r="B65" s="3">
+        <v>100101191251161</v>
+      </c>
+      <c r="C65" s="3">
         <v>622125105063</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E65" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J65" s="7"/>
+      <c r="E65" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J65" s="6"/>
+    </row>
+    <row r="66" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B66" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:B64">
+  <conditionalFormatting sqref="B3:B65">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>

</xml_diff>